<commit_message>
Implemented CarLotDAO.java with tests
</commit_message>
<xml_diff>
--- a/documentation/Database Design.xlsx
+++ b/documentation/Database Design.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\School\FL22\CSC251 - Adv Java\Group Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\School\FL22\CSC251 - Adv Java\Group Project\CSC251CarLotProject\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5B0EC92-9317-4163-9548-C9519872560A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50038C23-EC7A-42CF-B428-C4D659DA7348}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7834BEB5-AA27-4911-A043-EACBA9B58426}"/>
   </bookViews>
@@ -38,9 +38,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
   <si>
-    <t>Vehicle</t>
-  </si>
-  <si>
     <t>VIN: char(17)</t>
   </si>
   <si>
@@ -108,6 +105,9 @@
   </si>
   <si>
     <t>are under the CarLot table. These values will change from one purchase</t>
+  </si>
+  <si>
+    <t>Car</t>
   </si>
 </sst>
 </file>
@@ -947,7 +947,7 @@
   <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I30" sqref="I30:I31"/>
+      <selection activeCell="B6" sqref="B6:B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -967,7 +967,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="5.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="39" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B1" s="40"/>
       <c r="C1" s="40"/>
@@ -1012,7 +1012,7 @@
       <c r="F4" s="25"/>
       <c r="G4" s="25"/>
       <c r="H4" s="42" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I4" s="50"/>
       <c r="J4" s="25"/>
@@ -1020,7 +1020,7 @@
     <row r="5" spans="1:10" ht="14.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="22"/>
       <c r="B5" s="42" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="C5" s="43"/>
       <c r="D5" s="26"/>
@@ -1028,30 +1028,30 @@
       <c r="F5" s="26"/>
       <c r="G5" s="26"/>
       <c r="H5" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J5" s="25"/>
     </row>
     <row r="6" spans="1:10" ht="2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="22"/>
       <c r="B6" s="44" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C6" s="47" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D6" s="27"/>
       <c r="E6" s="28"/>
       <c r="F6" s="28"/>
       <c r="G6" s="28"/>
       <c r="H6" s="45" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I6" s="52" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J6" s="25"/>
     </row>
@@ -1095,7 +1095,7 @@
       <c r="A10" s="22"/>
       <c r="B10" s="4"/>
       <c r="C10" s="5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D10" s="34"/>
       <c r="E10" s="34"/>
@@ -1103,7 +1103,7 @@
       <c r="G10" s="34"/>
       <c r="H10" s="6"/>
       <c r="I10" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J10" s="25"/>
     </row>
@@ -1111,7 +1111,7 @@
       <c r="A11" s="22"/>
       <c r="B11" s="4"/>
       <c r="C11" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D11" s="34"/>
       <c r="E11" s="34"/>
@@ -1119,7 +1119,7 @@
       <c r="G11" s="34"/>
       <c r="H11" s="6"/>
       <c r="I11" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J11" s="25"/>
     </row>
@@ -1127,7 +1127,7 @@
       <c r="A12" s="22"/>
       <c r="B12" s="7"/>
       <c r="C12" s="8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D12" s="34"/>
       <c r="E12" s="34"/>
@@ -1135,7 +1135,7 @@
       <c r="G12" s="34"/>
       <c r="H12" s="6"/>
       <c r="I12" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J12" s="25"/>
     </row>
@@ -1149,7 +1149,7 @@
       <c r="G13" s="35"/>
       <c r="H13" s="9"/>
       <c r="I13" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J13" s="22"/>
     </row>
@@ -1163,7 +1163,7 @@
       <c r="G14" s="35"/>
       <c r="H14" s="9"/>
       <c r="I14" s="10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J14" s="22"/>
     </row>
@@ -1175,13 +1175,13 @@
       <c r="E15" s="25"/>
       <c r="F15" s="25"/>
       <c r="G15" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="H15" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="H15" s="11" t="s">
-        <v>17</v>
-      </c>
       <c r="I15" s="12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J15" s="22"/>
     </row>
@@ -1200,7 +1200,7 @@
     <row r="17" spans="1:10" ht="15.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A17" s="22"/>
       <c r="B17" s="36" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C17" s="37"/>
       <c r="D17" s="37"/>
@@ -1214,7 +1214,7 @@
     <row r="18" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="22"/>
       <c r="B18" s="14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C18" s="15"/>
       <c r="D18" s="15"/>
@@ -1228,7 +1228,7 @@
     <row r="19" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="22"/>
       <c r="B19" s="14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C19" s="15"/>
       <c r="D19" s="15"/>
@@ -1242,7 +1242,7 @@
     <row r="20" spans="1:10" ht="14.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="22"/>
       <c r="B20" s="14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C20" s="15"/>
       <c r="D20" s="15"/>
@@ -1256,7 +1256,7 @@
     <row r="21" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="22"/>
       <c r="B21" s="17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C21" s="13"/>
       <c r="D21" s="13"/>
@@ -1270,7 +1270,7 @@
     <row r="22" spans="1:10" ht="14.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="22"/>
       <c r="B22" s="19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C22" s="20"/>
       <c r="D22" s="20"/>

</xml_diff>